<commit_message>
updated Taganito location and Figure title
</commit_message>
<xml_diff>
--- a/Plants_Plot_Data.xlsx
+++ b/Plants_Plot_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/ericyo_ntnu_no/Documents/Nickel/Data and code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericyoung/Documents/GitHub/flying-dog-beers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72506BF6-CCF3-6B41-B341-4560E90C741B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A22233-F389-EC4C-AD1F-1F6FEB551481}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1420" windowWidth="27640" windowHeight="15720" xr2:uid="{9540A159-F7EA-7640-99CF-F24AEC0D86EC}"/>
+    <workbookView xWindow="3920" yWindow="-17940" windowWidth="27640" windowHeight="15720" xr2:uid="{9540A159-F7EA-7640-99CF-F24AEC0D86EC}"/>
   </bookViews>
   <sheets>
     <sheet name="PlotData" sheetId="1" r:id="rId1"/>
@@ -2280,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534F96EE-9650-F341-97AA-7C1F0BFFE551}">
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="DN1" sqref="DN1"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5860,7 +5860,7 @@
         <v>9.5397999999999996</v>
       </c>
       <c r="G75">
-        <v>25.811969999999999</v>
+        <v>125.81197</v>
       </c>
       <c r="H75" t="s">
         <v>448</v>

</xml_diff>